<commit_message>
Fixed alignment for databases tab
</commit_message>
<xml_diff>
--- a/SQLInstance/Synapse Compatibility Checks.xlsx
+++ b/SQLInstance/Synapse Compatibility Checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/silvam_microsoft_com/Documents/Projects/GitHub/SynapseCompatibilityChecks/SQLInstance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="647" documentId="11_F25DC773A252ABDACC104855719E50C65ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B031F12-1778-4F75-9C4B-BA66D62A55E3}"/>
+  <xr:revisionPtr revIDLastSave="649" documentId="11_F25DC773A252ABDACC104855719E50C65ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B1E8480-0172-4424-ABB5-A859CE4C7810}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instance" sheetId="15" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="131">
   <si>
     <t>DatabaseName</t>
   </si>
@@ -560,7 +560,25 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1189,7 +1207,7 @@
   <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{D1F0D0B2-4B09-4EE8-9D7B-867FA5F3FF31}" name="ServerName"/>
     <tableColumn id="2" xr3:uid="{542398CE-8D7E-4464-80AF-5F23B41FDE13}" name="WindowsRelease"/>
-    <tableColumn id="3" xr3:uid="{467B99FC-EDAA-4077-87AD-A16B53ABC49F}" name="CreatedDate" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{467B99FC-EDAA-4077-87AD-A16B53ABC49F}" name="CreatedDate" dataDxfId="40"/>
     <tableColumn id="4" xr3:uid="{FEDC7504-54DD-4858-95A6-8B26A71DEA20}" name="Version"/>
     <tableColumn id="5" xr3:uid="{9E3A32DA-28D2-4FFE-82AD-1FEDCBA265DF}" name="Edition"/>
     <tableColumn id="6" xr3:uid="{9D4074F1-0FA1-4540-A724-4086C486CD58}" name="ProductLevel"/>
@@ -1279,41 +1297,42 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{04934680-DE44-4658-8EEE-EE198E645418}" name="Table15" displayName="Table15" ref="A1:AF3" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <autoFilter ref="A1:AF3" xr:uid="{04934680-DE44-4658-8EEE-EE198E645418}"/>
-  <tableColumns count="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{04934680-DE44-4658-8EEE-EE198E645418}" name="Table15" displayName="Table15" ref="A1:AG3" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A1:AG3" xr:uid="{04934680-DE44-4658-8EEE-EE198E645418}"/>
+  <tableColumns count="33">
     <tableColumn id="1" xr3:uid="{08FC8CC8-E7B8-4816-977B-9CB62A890F89}" name="DatabaseName"/>
-    <tableColumn id="2" xr3:uid="{9D6B53AF-2D5D-4726-9A05-26B98F548FA9}" name="DataMB" dataDxfId="36" dataCellStyle="Comma"/>
-    <tableColumn id="32" xr3:uid="{8001F6BF-FFC7-4041-B201-37565753B71E}" name="Files" dataDxfId="35" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{F94A5334-ABE9-4616-B743-6C286E4DEA62}" name="Tables" dataDxfId="34" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{0C7F4299-0D10-4B95-AFC8-8C841D67C4AD}" name="Empty" dataDxfId="33" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{3C279FE9-99FC-438C-B012-86C010D4FDF7}" name="Small" dataDxfId="32" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{DC638AD7-DC7C-49AE-B6A1-79671D34F937}" name="Medium" dataDxfId="31" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{3D592ACD-58E8-4828-8B1F-BC7981CF87E3}" name="Large" dataDxfId="30" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{E0C74F65-5AD9-47DC-B91B-1C35532A968C}" name="VeryLarge" dataDxfId="29" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{3C5F7A9B-894A-4AD9-9329-9999A5113B11}" name="Columns" dataDxfId="28" dataCellStyle="Comma"/>
-    <tableColumn id="10" xr3:uid="{48FAE5BC-97D9-48E3-85EF-3BBFCEC46B3A}" name="Rows" dataDxfId="27"/>
-    <tableColumn id="11" xr3:uid="{24E93FD5-32C2-4CCC-9E21-0D0C9F19FFD3}" name="Views" dataDxfId="26"/>
-    <tableColumn id="12" xr3:uid="{A8D1FCF8-FE92-41DD-A87D-35DC3CE62010}" name="Procs" dataDxfId="25"/>
-    <tableColumn id="13" xr3:uid="{D951C168-B143-4ACC-85C6-E0957B6EDB3E}" name="Functions" dataDxfId="24"/>
-    <tableColumn id="14" xr3:uid="{72F0D9C8-2DE8-48C8-9686-F9F4ED01EC64}" name="Indexes" dataDxfId="23"/>
-    <tableColumn id="15" xr3:uid="{14C70B61-31E5-439B-B780-80F5F05BD484}" name="ColumnStores" dataDxfId="22"/>
-    <tableColumn id="16" xr3:uid="{63E3DEC7-B586-4449-98F1-6B590AC00B4B}" name="UniqueIndexes" dataDxfId="21"/>
-    <tableColumn id="17" xr3:uid="{D6F46219-F48C-4132-9C04-4C34B20F7FF7}" name="IncludedColumnIndexes" dataDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{B77BDD42-7E17-48BE-9D68-B9C564FB4E2E}" name="LargeTextColumns" dataDxfId="19"/>
-    <tableColumn id="19" xr3:uid="{A9F0C99F-143B-4188-AB60-8A5A9111F0EA}" name="IncompatibleDefaults" dataDxfId="18"/>
-    <tableColumn id="20" xr3:uid="{E20F4597-BE89-4D71-8E04-6FAF49B561FB}" name="FilteredIndexes" dataDxfId="17"/>
-    <tableColumn id="21" xr3:uid="{A568CA2C-4FE1-4B8A-95BE-E5023214150A}" name="ComputedColumns" dataDxfId="16"/>
-    <tableColumn id="22" xr3:uid="{3D403AA1-BF84-4B47-AEC9-4B6712F4E39A}" name="XServerRoutines" dataDxfId="15"/>
-    <tableColumn id="23" xr3:uid="{62DE4B32-328C-4156-83BF-023D25D01BE7}" name="XOutRoutines" dataDxfId="14"/>
-    <tableColumn id="24" xr3:uid="{065DA0B8-B7B8-4E62-B5C1-D5749AD66E9D}" name="XOutDbs" dataDxfId="13"/>
-    <tableColumn id="25" xr3:uid="{E0E46443-7A15-41DE-A8F4-070139F2C237}" name="XInRoutines" dataDxfId="12"/>
-    <tableColumn id="26" xr3:uid="{48B27011-FBAA-4436-A37F-76514D53F206}" name="XInDbs" dataDxfId="11"/>
-    <tableColumn id="27" xr3:uid="{C5F813C2-D758-4668-994B-4493EC0FCFB7}" name="UsesForXML" dataDxfId="10"/>
-    <tableColumn id="28" xr3:uid="{914CD33C-7704-46B9-8B1F-F85F52818C50}" name="UsesCursor" dataDxfId="9"/>
-    <tableColumn id="29" xr3:uid="{F83C3FEE-DE98-4300-BA6D-B7A42F5AE4FC}" name="IncompatibleColumns" dataDxfId="8"/>
-    <tableColumn id="30" xr3:uid="{868B6C8E-AE03-4F1A-94F1-BF5DBBDB1ECD}" name="IncompatibleRoutinesByType" dataDxfId="7"/>
-    <tableColumn id="31" xr3:uid="{484AA305-68C7-4207-A121-97107E95660A}" name="Sequences" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{9D6B53AF-2D5D-4726-9A05-26B98F548FA9}" name="DataMB" dataDxfId="37" dataCellStyle="Comma"/>
+    <tableColumn id="32" xr3:uid="{8001F6BF-FFC7-4041-B201-37565753B71E}" name="Files" dataDxfId="36" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{F94A5334-ABE9-4616-B743-6C286E4DEA62}" name="Tables" dataDxfId="35" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{0C7F4299-0D10-4B95-AFC8-8C841D67C4AD}" name="Empty" dataDxfId="34" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{3C279FE9-99FC-438C-B012-86C010D4FDF7}" name="Small" dataDxfId="33" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{DC638AD7-DC7C-49AE-B6A1-79671D34F937}" name="Medium" dataDxfId="32" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{3D592ACD-58E8-4828-8B1F-BC7981CF87E3}" name="Large" dataDxfId="31" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{E0C74F65-5AD9-47DC-B91B-1C35532A968C}" name="VeryLarge" dataDxfId="30" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{3C5F7A9B-894A-4AD9-9329-9999A5113B11}" name="Columns" dataDxfId="29" dataCellStyle="Comma"/>
+    <tableColumn id="10" xr3:uid="{48FAE5BC-97D9-48E3-85EF-3BBFCEC46B3A}" name="Rows" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{24E93FD5-32C2-4CCC-9E21-0D0C9F19FFD3}" name="Views" dataDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{A8D1FCF8-FE92-41DD-A87D-35DC3CE62010}" name="Procs" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{D951C168-B143-4ACC-85C6-E0957B6EDB3E}" name="Functions" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{72F0D9C8-2DE8-48C8-9686-F9F4ED01EC64}" name="Indexes" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{14C70B61-31E5-439B-B780-80F5F05BD484}" name="ColumnStores" dataDxfId="23"/>
+    <tableColumn id="16" xr3:uid="{63E3DEC7-B586-4449-98F1-6B590AC00B4B}" name="UniqueIndexes" dataDxfId="22"/>
+    <tableColumn id="17" xr3:uid="{D6F46219-F48C-4132-9C04-4C34B20F7FF7}" name="IncludedColumnIndexes" dataDxfId="21"/>
+    <tableColumn id="18" xr3:uid="{B77BDD42-7E17-48BE-9D68-B9C564FB4E2E}" name="LargeTextColumns" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{A9F0C99F-143B-4188-AB60-8A5A9111F0EA}" name="IncompatibleDefaults" dataDxfId="19"/>
+    <tableColumn id="20" xr3:uid="{E20F4597-BE89-4D71-8E04-6FAF49B561FB}" name="FilteredIndexes" dataDxfId="18"/>
+    <tableColumn id="21" xr3:uid="{A568CA2C-4FE1-4B8A-95BE-E5023214150A}" name="ComputedColumns" dataDxfId="17"/>
+    <tableColumn id="22" xr3:uid="{3D403AA1-BF84-4B47-AEC9-4B6712F4E39A}" name="XServerRoutines" dataDxfId="16"/>
+    <tableColumn id="33" xr3:uid="{D059724C-E9BB-4291-9FAE-A107BC0A732D}" name="LinkedServers" dataDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{62DE4B32-328C-4156-83BF-023D25D01BE7}" name="XOutRoutines" dataDxfId="15"/>
+    <tableColumn id="24" xr3:uid="{065DA0B8-B7B8-4E62-B5C1-D5749AD66E9D}" name="XOutDbs" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{E0E46443-7A15-41DE-A8F4-070139F2C237}" name="XInRoutines" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{48B27011-FBAA-4436-A37F-76514D53F206}" name="XInDbs" dataDxfId="12"/>
+    <tableColumn id="27" xr3:uid="{C5F813C2-D758-4668-994B-4493EC0FCFB7}" name="UsesForXML" dataDxfId="11"/>
+    <tableColumn id="28" xr3:uid="{914CD33C-7704-46B9-8B1F-F85F52818C50}" name="UsesCursor" dataDxfId="10"/>
+    <tableColumn id="29" xr3:uid="{F83C3FEE-DE98-4300-BA6D-B7A42F5AE4FC}" name="IncompatibleColumns" dataDxfId="9"/>
+    <tableColumn id="30" xr3:uid="{868B6C8E-AE03-4F1A-94F1-BF5DBBDB1ECD}" name="IncompatibleRoutinesByType" dataDxfId="8"/>
+    <tableColumn id="31" xr3:uid="{484AA305-68C7-4207-A121-97107E95660A}" name="Sequences" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1327,15 +1346,15 @@
     <tableColumn id="2" xr3:uid="{1C838312-A5EF-4751-8D1D-F825767EF6E7}" name="SchemaName"/>
     <tableColumn id="3" xr3:uid="{5CFB7B13-55FD-468D-A771-603D8780494F}" name="ObjectName"/>
     <tableColumn id="4" xr3:uid="{76CA0F41-FB30-485F-991E-8EE447313AD0}" name="RowCount"/>
-    <tableColumn id="5" xr3:uid="{8C7937F6-A34F-4294-BA33-C82DCB6DD32A}" name="RowLength" dataDxfId="5" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{8C7937F6-A34F-4294-BA33-C82DCB6DD32A}" name="RowLength" dataDxfId="6" dataCellStyle="Comma"/>
     <tableColumn id="6" xr3:uid="{0276EFED-0031-48CC-B6ED-40A11B5DF85A}" name="PK"/>
     <tableColumn id="7" xr3:uid="{F7F24CC7-3DAD-47BD-B6F3-4FE386938ED2}" name="PKType"/>
     <tableColumn id="8" xr3:uid="{7F3D37D0-6270-4708-818E-4CD18E46EA29}" name="Writes"/>
     <tableColumn id="9" xr3:uid="{4D327070-572D-4AF1-A075-9097A49E5A86}" name="Reads"/>
-    <tableColumn id="10" xr3:uid="{75FF4492-DB58-4724-B519-E367FE1E8179}" name="PKCols" dataDxfId="4" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{2E87D210-ABF3-4464-A4DC-16B74E89BDB6}" name="Indexes" dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{1668BDC5-975B-4873-9AC5-5D5BCFF3FD47}" name="Reserved_Size_Mbs" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="13" xr3:uid="{2832FA48-B057-4989-BF87-A30C84157A3E}" name="Used_Size_Mbs" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="10" xr3:uid="{75FF4492-DB58-4724-B519-E367FE1E8179}" name="PKCols" dataDxfId="5" dataCellStyle="Comma"/>
+    <tableColumn id="11" xr3:uid="{2E87D210-ABF3-4464-A4DC-16B74E89BDB6}" name="Indexes" dataDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{1668BDC5-975B-4873-9AC5-5D5BCFF3FD47}" name="Reserved_Size_Mbs" dataDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="13" xr3:uid="{2832FA48-B057-4989-BF87-A30C84157A3E}" name="Used_Size_Mbs" dataDxfId="2" dataCellStyle="Comma"/>
     <tableColumn id="17" xr3:uid="{6FEAA87B-CF4B-4E7C-A8EB-59FF9CDC8F54}" name="ColumnStores"/>
     <tableColumn id="18" xr3:uid="{789B2956-CC68-46BE-85DE-D109ECA7F626}" name="ColumnsCount"/>
     <tableColumn id="19" xr3:uid="{8FD2F1D2-178E-496E-8940-78D395BE683A}" name="HasIdentity"/>
@@ -1419,7 +1438,7 @@
     <tableColumn id="8" xr3:uid="{5200B7E2-4A03-490D-B193-82BDCAF67D3B}" name="UsesForXML"/>
     <tableColumn id="9" xr3:uid="{9D4849EA-A44C-4263-8AAA-870299FBF02A}" name="UsesCursor"/>
     <tableColumn id="11" xr3:uid="{2C3AB52A-C0EF-44E9-B19D-6C30F9F492DD}" name="IncompatibleType"/>
-    <tableColumn id="10" xr3:uid="{95203223-D59C-49A6-8119-D5B872A7DD18}" name="ROUTINE_DEFINITION" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{95203223-D59C-49A6-8119-D5B872A7DD18}" name="ROUTINE_DEFINITION" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1690,7 +1709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E30F4C-CF63-4D1D-96BF-CA0D8DEE5EAA}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -2007,11 +2026,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X13" sqref="X13"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2038,18 +2057,19 @@
     <col min="21" max="21" width="21.453125" style="3" customWidth="1"/>
     <col min="22" max="22" width="20.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.54296875" style="3" customWidth="1"/>
-    <col min="25" max="25" width="24.54296875" style="3" customWidth="1"/>
-    <col min="26" max="26" width="24.54296875" style="4" customWidth="1"/>
-    <col min="27" max="27" width="23" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.1796875" style="3" customWidth="1"/>
+    <col min="25" max="25" width="16.54296875" style="3" customWidth="1"/>
+    <col min="26" max="26" width="24.54296875" style="3" customWidth="1"/>
+    <col min="27" max="27" width="24.54296875" style="4" customWidth="1"/>
+    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2120,47 +2140,51 @@
         <v>70</v>
       </c>
       <c r="X1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="7"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
@@ -2172,6 +2196,7 @@
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>